<commit_message>
all modeling procedure is done
</commit_message>
<xml_diff>
--- a/archived modeled files/Severn River/Raw and un-modeled excel files to be run by WATUM/Dx_1998_Li_et_al_Paper02_Severn.xlsx
+++ b/archived modeled files/Severn River/Raw and un-modeled excel files to be run by WATUM/Dx_1998_Li_et_al_Paper02_Severn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="63900" windowWidth="14805" windowHeight="7335"/>
   </bookViews>
   <sheets>
     <sheet name="Setting" sheetId="8" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="121">
   <si>
     <t>Project Name</t>
   </si>
@@ -437,9 +437,6 @@
     <t>St7 @ 13.775 (km)</t>
   </si>
   <si>
-    <t>Li et al. 2 (1998)</t>
-  </si>
-  <si>
     <t>None Dispersive Model</t>
   </si>
   <si>
@@ -456,6 +453,21 @@
   </si>
   <si>
     <t>Li et al. (1998) [1]</t>
+  </si>
+  <si>
+    <t>Li et al (1998)</t>
+  </si>
+  <si>
+    <t>Li et al 2 (1998)</t>
+  </si>
+  <si>
+    <t>Deng et al (2001)</t>
+  </si>
+  <si>
+    <t>Disley et al (2015)</t>
+  </si>
+  <si>
+    <t>Noori et al (2017)</t>
   </si>
 </sst>
 </file>
@@ -1403,7 +1415,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1465,7 +1477,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="29" fillId="37" borderId="11" xfId="37" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1503,9 +1514,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="38" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1675,6 +1683,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="32" borderId="7" xfId="37" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4685,20 +4696,20 @@
   </sheetPr>
   <dimension ref="A1:X91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="55.85546875" style="56" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" style="54" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="48"/>
+      <c r="B1" s="46"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -4726,7 +4737,7 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="49" t="str">
+      <c r="B2" s="47" t="str">
         <f ca="1">MID(CELL("filename"),SEARCH("[",CELL("filename"))+1, SEARCH("]",CELL("filename"))-SEARCH("[",CELL("filename"))-1)</f>
         <v>Dx_1998_Li_et_al_Paper02_Severn.xlsx</v>
       </c>
@@ -4757,7 +4768,7 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="88">
+      <c r="B3" s="86">
         <f>DATE(2019,1,10)</f>
         <v>43475</v>
       </c>
@@ -4788,7 +4799,7 @@
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="47" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="5"/>
@@ -4818,7 +4829,7 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="5"/>
@@ -4848,7 +4859,7 @@
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="50" t="str">
+      <c r="B6" s="48" t="str">
         <f ca="1">LEFT(CELL("filename"),FIND("[",CELL("filename"),1)-1)</f>
         <v>C:\Users\Mostafa\Desktop\watum_Working_Branch\</v>
       </c>
@@ -4877,7 +4888,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
-      <c r="B7" s="51"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -4905,7 +4916,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="48"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -4933,8 +4944,8 @@
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="52">
-        <v>60</v>
+      <c r="B9" s="50">
+        <v>20</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -4963,8 +4974,8 @@
       <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="54">
-        <v>15</v>
+      <c r="B10" s="99">
+        <v>10</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -4993,8 +5004,8 @@
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="53" t="s">
-        <v>93</v>
+      <c r="B11" s="51" t="s">
+        <v>116</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -5023,7 +5034,7 @@
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="52">
+      <c r="B12" s="50">
         <v>50</v>
       </c>
       <c r="C12" s="5"/>
@@ -5053,7 +5064,7 @@
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="54">
+      <c r="B13" s="52">
         <v>0</v>
       </c>
       <c r="C13" s="5"/>
@@ -5083,7 +5094,7 @@
       <c r="A14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="52">
+      <c r="B14" s="50">
         <v>0.5</v>
       </c>
       <c r="C14" s="5"/>
@@ -5111,7 +5122,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="51"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -5137,7 +5148,7 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="51"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -5163,7 +5174,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="B17" s="51"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -5189,7 +5200,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
-      <c r="B18" s="51"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -5215,7 +5226,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="51"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -5241,7 +5252,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="55"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -5267,7 +5278,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
-      <c r="B21" s="51"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -5293,7 +5304,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="B22" s="51"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -5319,7 +5330,7 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
-      <c r="B23" s="51"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -5345,7 +5356,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
-      <c r="B24" s="51"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -5371,7 +5382,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
-      <c r="B25" s="51"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -5397,7 +5408,7 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
-      <c r="B26" s="51"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -5423,7 +5434,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
-      <c r="B27" s="51"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -5449,7 +5460,7 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
-      <c r="B28" s="51"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -5475,7 +5486,7 @@
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
-      <c r="B29" s="51"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -5501,7 +5512,7 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
-      <c r="B30" s="51"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -5527,7 +5538,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
-      <c r="B31" s="51"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -5553,7 +5564,7 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
-      <c r="B32" s="51"/>
+      <c r="B32" s="49"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -5579,7 +5590,7 @@
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
-      <c r="B33" s="51"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -5605,7 +5616,7 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
-      <c r="B34" s="51"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -5631,7 +5642,7 @@
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
-      <c r="B35" s="51"/>
+      <c r="B35" s="49"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -5657,7 +5668,7 @@
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
-      <c r="B36" s="51"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
@@ -5683,7 +5694,7 @@
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
-      <c r="B37" s="51"/>
+      <c r="B37" s="49"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
@@ -5709,7 +5720,7 @@
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
-      <c r="B38" s="51"/>
+      <c r="B38" s="49"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
@@ -5735,7 +5746,7 @@
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
-      <c r="B39" s="51"/>
+      <c r="B39" s="49"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
@@ -5761,7 +5772,7 @@
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
-      <c r="B40" s="51"/>
+      <c r="B40" s="49"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
@@ -5787,7 +5798,7 @@
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
-      <c r="B41" s="51"/>
+      <c r="B41" s="49"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
@@ -5813,7 +5824,7 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
-      <c r="B42" s="51"/>
+      <c r="B42" s="49"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -5839,7 +5850,7 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
-      <c r="B43" s="51"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -5865,7 +5876,7 @@
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
-      <c r="B44" s="51"/>
+      <c r="B44" s="49"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
@@ -5891,7 +5902,7 @@
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
-      <c r="B45" s="51"/>
+      <c r="B45" s="49"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -5917,7 +5928,7 @@
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
-      <c r="B46" s="51"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -5943,7 +5954,7 @@
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
-      <c r="B47" s="51"/>
+      <c r="B47" s="49"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -5969,7 +5980,7 @@
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
-      <c r="B48" s="51"/>
+      <c r="B48" s="49"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
@@ -5995,7 +6006,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
-      <c r="B49" s="51"/>
+      <c r="B49" s="49"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
@@ -6021,7 +6032,7 @@
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
-      <c r="B50" s="51"/>
+      <c r="B50" s="49"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
@@ -6047,7 +6058,7 @@
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
-      <c r="B51" s="51"/>
+      <c r="B51" s="49"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
@@ -6073,7 +6084,7 @@
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
-      <c r="B52" s="51"/>
+      <c r="B52" s="49"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
@@ -6099,7 +6110,7 @@
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
-      <c r="B53" s="51"/>
+      <c r="B53" s="49"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -6125,7 +6136,7 @@
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
-      <c r="B54" s="51"/>
+      <c r="B54" s="49"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
@@ -6151,7 +6162,7 @@
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
-      <c r="B55" s="51"/>
+      <c r="B55" s="49"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
@@ -6177,7 +6188,7 @@
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
-      <c r="B56" s="51"/>
+      <c r="B56" s="49"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
@@ -6203,7 +6214,7 @@
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
-      <c r="B57" s="51"/>
+      <c r="B57" s="49"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
@@ -6229,7 +6240,7 @@
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
-      <c r="B58" s="51"/>
+      <c r="B58" s="49"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
@@ -6255,7 +6266,7 @@
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
-      <c r="B59" s="51"/>
+      <c r="B59" s="49"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
@@ -6281,7 +6292,7 @@
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
-      <c r="B60" s="51"/>
+      <c r="B60" s="49"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
@@ -6307,7 +6318,7 @@
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="9"/>
-      <c r="B61" s="51"/>
+      <c r="B61" s="49"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
@@ -6333,7 +6344,7 @@
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="9"/>
-      <c r="B62" s="51"/>
+      <c r="B62" s="49"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
@@ -6359,7 +6370,7 @@
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="9"/>
-      <c r="B63" s="51"/>
+      <c r="B63" s="49"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
@@ -7093,46 +7104,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="62" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="62" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="62" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="62" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="62" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="62" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="62" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" style="62" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" style="62" customWidth="1"/>
-    <col min="11" max="12" width="19.140625" style="62" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="62" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="62" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" style="62" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" style="62" customWidth="1"/>
-    <col min="17" max="17" width="39.7109375" style="62" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" style="62" customWidth="1"/>
-    <col min="19" max="19" width="22.5703125" style="62" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="62"/>
-    <col min="21" max="21" width="21.42578125" style="62" customWidth="1"/>
-    <col min="22" max="22" width="38.5703125" style="62" customWidth="1"/>
-    <col min="23" max="23" width="29.42578125" style="62" customWidth="1"/>
-    <col min="24" max="24" width="41.140625" style="63" customWidth="1"/>
-    <col min="25" max="25" width="17.140625" style="64" customWidth="1"/>
-    <col min="26" max="27" width="19.42578125" style="62" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" style="62" customWidth="1"/>
-    <col min="29" max="30" width="12.140625" style="62" customWidth="1"/>
-    <col min="31" max="31" width="11.140625" style="62" customWidth="1"/>
-    <col min="32" max="34" width="12.28515625" style="62" customWidth="1"/>
-    <col min="35" max="35" width="11.140625" style="62" customWidth="1"/>
-    <col min="36" max="36" width="9.140625" style="62"/>
-    <col min="37" max="37" width="12.28515625" style="62" customWidth="1"/>
-    <col min="38" max="39" width="11.140625" style="62" customWidth="1"/>
-    <col min="40" max="40" width="9.140625" style="62"/>
-    <col min="41" max="41" width="30.140625" style="62" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="26.5703125" style="62" bestFit="1" customWidth="1"/>
-    <col min="43" max="16384" width="9.140625" style="62"/>
+    <col min="1" max="1" width="23.28515625" style="60" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="60" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="60" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="60" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="60" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="60" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="60" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="60" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" style="60" customWidth="1"/>
+    <col min="11" max="12" width="19.140625" style="60" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="60" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="60" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" style="60" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" style="60" customWidth="1"/>
+    <col min="17" max="17" width="39.7109375" style="60" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" style="60" customWidth="1"/>
+    <col min="19" max="19" width="22.5703125" style="60" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="60"/>
+    <col min="21" max="21" width="21.42578125" style="60" customWidth="1"/>
+    <col min="22" max="22" width="38.5703125" style="60" customWidth="1"/>
+    <col min="23" max="23" width="29.42578125" style="60" customWidth="1"/>
+    <col min="24" max="24" width="41.140625" style="61" customWidth="1"/>
+    <col min="25" max="25" width="17.140625" style="62" customWidth="1"/>
+    <col min="26" max="27" width="19.42578125" style="60" customWidth="1"/>
+    <col min="28" max="28" width="16.42578125" style="60" customWidth="1"/>
+    <col min="29" max="30" width="12.140625" style="60" customWidth="1"/>
+    <col min="31" max="31" width="11.140625" style="60" customWidth="1"/>
+    <col min="32" max="34" width="12.28515625" style="60" customWidth="1"/>
+    <col min="35" max="35" width="11.140625" style="60" customWidth="1"/>
+    <col min="36" max="36" width="9.140625" style="60"/>
+    <col min="37" max="37" width="12.28515625" style="60" customWidth="1"/>
+    <col min="38" max="39" width="11.140625" style="60" customWidth="1"/>
+    <col min="40" max="40" width="9.140625" style="60"/>
+    <col min="41" max="41" width="30.140625" style="60" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="26.5703125" style="60" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="9.140625" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="66" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="64" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>40</v>
       </c>
@@ -7202,8 +7213,8 @@
       <c r="W1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="95" t="s">
-        <v>115</v>
+      <c r="X1" s="93" t="s">
+        <v>114</v>
       </c>
       <c r="Y1" s="17" t="s">
         <v>45</v>
@@ -7214,13 +7225,13 @@
       <c r="AA1" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="AB1" s="26" t="s">
+      <c r="AB1" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="AC1" s="26" t="s">
+      <c r="AC1" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="AD1" s="26" t="s">
+      <c r="AD1" s="25" t="s">
         <v>74</v>
       </c>
       <c r="AE1" s="18" t="s">
@@ -7250,1008 +7261,1008 @@
       <c r="AM1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="AN1" s="65" t="s">
+      <c r="AN1" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="AO1" s="98" t="s">
+      <c r="AO1" s="96" t="s">
+        <v>112</v>
+      </c>
+      <c r="AP1" s="96" t="s">
         <v>113</v>
       </c>
-      <c r="AP1" s="98" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:42" s="75" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+    </row>
+    <row r="2" spans="1:42" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="71">
+      <c r="B2" s="69">
         <v>0</v>
       </c>
-      <c r="C2" s="71">
+      <c r="C2" s="69">
         <v>210</v>
       </c>
-      <c r="D2" s="71">
+      <c r="D2" s="69">
         <v>7.33</v>
       </c>
-      <c r="E2" s="71">
+      <c r="E2" s="69">
         <f>(1/5)*(0.3)*1000/3600</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="F2" s="71">
+      <c r="F2" s="69">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="G2" s="71">
+      <c r="G2" s="69">
         <f>(1/5)*(2.35)*1000/3600</f>
         <v>0.13055555555555556</v>
       </c>
-      <c r="H2" s="71">
+      <c r="H2" s="69">
         <v>7.33</v>
       </c>
-      <c r="I2" s="71"/>
-      <c r="J2" s="72">
+      <c r="I2" s="69"/>
+      <c r="J2" s="70">
         <f>142.8/10000</f>
         <v>1.4280000000000001E-2</v>
       </c>
-      <c r="K2" s="72">
+      <c r="K2" s="70">
         <v>0.46241399999999999</v>
       </c>
-      <c r="L2" s="72">
+      <c r="L2" s="70">
         <v>17.486969999999999</v>
       </c>
-      <c r="M2" s="72">
+      <c r="M2" s="70">
         <v>1.0510314000000001</v>
       </c>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="74">
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="72">
         <f>Table1[Q '[m3/sec']]/(Table1[depth '[meters']]*Table1[width '[meters']])</f>
         <v>0.90648043593010741</v>
       </c>
-      <c r="R2" s="75">
+      <c r="R2" s="73">
         <f>(Table1[[#This Row],[Reach Length '[meters']]]/(Table1[[#This Row],[Q '[m3/sec']]]/(Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]])))/3600</f>
         <v>6.4351453182196455E-2</v>
       </c>
-      <c r="S2" s="75">
+      <c r="S2" s="73">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
         <v>0.70028011204481799</v>
       </c>
-      <c r="T2" s="75">
+      <c r="T2" s="73">
         <v>1</v>
       </c>
-      <c r="U2" s="75">
+      <c r="U2" s="73">
         <v>0</v>
       </c>
-      <c r="V2" s="75">
+      <c r="V2" s="73">
         <v>0</v>
       </c>
-      <c r="W2" s="75">
+      <c r="W2" s="73">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>0.21</v>
       </c>
-      <c r="X2" s="96">
+      <c r="X2" s="94">
         <v>1.0510314000000001</v>
       </c>
-      <c r="Y2" s="76" t="str">
+      <c r="Y2" s="74" t="str">
         <f>IF(AVERAGE(Table1[[#This Row],[Error Ti]]&lt;=AVERAGE(Table1[[#This Row],[Error Tp]])),"use Ti","use Tp")</f>
         <v>use Ti</v>
       </c>
-      <c r="Z2" s="75">
+      <c r="Z2" s="73">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]-Table1[[#This Row],[Start point distance '[meters']]]</f>
         <v>210</v>
       </c>
-      <c r="AA2" s="75">
+      <c r="AA2" s="73">
         <f>(Table1[[#This Row],[Tp]]-AN2)*3600</f>
         <v>299.88</v>
       </c>
-      <c r="AB2" s="77">
+      <c r="AB2" s="75">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>19</v>
-      </c>
-      <c r="AC2" s="77">
+        <v>29</v>
+      </c>
+      <c r="AC2" s="75">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>3.5</v>
-      </c>
-      <c r="AD2" s="77">
+        <v>10.5</v>
+      </c>
+      <c r="AD2" s="75">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
         <v>0</v>
       </c>
-      <c r="AE2" s="75">
+      <c r="AE2" s="73">
         <f t="shared" ref="AE2:AE3" si="0">Delta_T__seconds</f>
-        <v>15</v>
-      </c>
-      <c r="AF2" s="76">
+        <v>10</v>
+      </c>
+      <c r="AF2" s="74">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
         <v>-2.8610871909317876</v>
       </c>
-      <c r="AG2" s="76">
+      <c r="AG2" s="74">
         <f>(('Reach Propertise'!$F2-'Reach Propertise'!$R2)/'Reach Propertise'!$F2)</f>
         <v>0.22747355123413618</v>
       </c>
-      <c r="AH2" s="76">
+      <c r="AH2" s="74">
         <f>((Table1[[#This Row],[Tt]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Tt]])</f>
         <v>0.507095252221474</v>
       </c>
-      <c r="AI2" s="78">
+      <c r="AI2" s="76">
         <f>Table1[[#This Row],[width '[meters']]]/Table1[[#This Row],[depth '[meters']]]</f>
         <v>37.816696726310191</v>
       </c>
-      <c r="AJ2" s="75">
+      <c r="AJ2" s="73">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>485.17318473479997</v>
-      </c>
-      <c r="AK2" s="75">
+        <v>161.72439491159997</v>
+      </c>
+      <c r="AK2" s="73">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="AL2" s="75">
+      <c r="AL2" s="73">
         <v>0</v>
       </c>
-      <c r="AM2" s="75">
+      <c r="AM2" s="73">
         <f>'Reach Propertise'!$F2</f>
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="AN2" s="75">
+      <c r="AN2" s="73">
         <v>0</v>
       </c>
-      <c r="AO2" s="99">
+      <c r="AO2" s="97">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>3</v>
-      </c>
-      <c r="AP2" s="99">
+        <v>10</v>
+      </c>
+      <c r="AP2" s="97">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:42" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+    <row r="3" spans="1:42" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="71">
+      <c r="B3" s="69">
         <v>210</v>
       </c>
-      <c r="C3" s="71">
+      <c r="C3" s="69">
         <v>1175</v>
       </c>
-      <c r="D3" s="71">
+      <c r="D3" s="69">
         <v>7.03</v>
       </c>
-      <c r="E3" s="71">
+      <c r="E3" s="69">
         <f>1.25*1000/3600</f>
         <v>0.34722222222222221</v>
       </c>
-      <c r="F3" s="71">
+      <c r="F3" s="69">
         <v>0.43330000000000002</v>
       </c>
-      <c r="G3" s="71">
+      <c r="G3" s="69">
         <f>5.15*1000/3600</f>
         <v>1.4305555555555556</v>
       </c>
-      <c r="H3" s="71">
+      <c r="H3" s="69">
         <v>7.03</v>
       </c>
-      <c r="I3" s="71"/>
-      <c r="J3" s="72">
+      <c r="I3" s="69"/>
+      <c r="J3" s="70">
         <f>51.81/10000</f>
         <v>5.1809999999999998E-3</v>
       </c>
-      <c r="K3" s="72">
+      <c r="K3" s="70">
         <v>0.38552900000000001</v>
       </c>
-      <c r="L3" s="72">
+      <c r="L3" s="70">
         <v>17.581569999999999</v>
       </c>
-      <c r="M3" s="72">
+      <c r="M3" s="70">
         <v>0.22527449999999999</v>
       </c>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="74">
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="72">
         <f>Table1[Q '[m3/sec']]/(Table1[depth '[meters']]*Table1[width '[meters']])</f>
         <v>1.0371477250592951</v>
       </c>
-      <c r="R3" s="75">
+      <c r="R3" s="73">
         <f>(Table1[[#This Row],[Reach Length '[meters']]]/(Table1[[#This Row],[Q '[m3/sec']]]/(Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]])))/3600</f>
         <v>0.25845455674140388</v>
       </c>
-      <c r="S3" s="75">
+      <c r="S3" s="73">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
         <v>0.75326307151832184</v>
       </c>
-      <c r="T3" s="75">
+      <c r="T3" s="73">
         <v>1</v>
       </c>
-      <c r="U3" s="75">
+      <c r="U3" s="73">
         <v>0</v>
       </c>
-      <c r="V3" s="75">
+      <c r="V3" s="73">
         <v>0</v>
       </c>
-      <c r="W3" s="75">
+      <c r="W3" s="73">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>1.175</v>
       </c>
-      <c r="X3" s="96">
+      <c r="X3" s="94">
         <v>0.22527449999999999</v>
       </c>
-      <c r="Y3" s="76" t="str">
+      <c r="Y3" s="74" t="str">
         <f>IF(AVERAGE(Table1[[#This Row],[Error Ti]]&lt;=AVERAGE(Table1[[#This Row],[Error Tp]])),"use Ti","use Tp")</f>
         <v>use Ti</v>
       </c>
-      <c r="Z3" s="75">
+      <c r="Z3" s="73">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]-Table1[[#This Row],[Start point distance '[meters']]]</f>
         <v>965</v>
       </c>
-      <c r="AA3" s="75">
+      <c r="AA3" s="73">
         <f>(Table1[[#This Row],[Tp]]-AN3)*3600</f>
         <v>-2040.12</v>
       </c>
-      <c r="AB3" s="77">
+      <c r="AB3" s="75">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>103</v>
-      </c>
-      <c r="AC3" s="77">
+        <v>155</v>
+      </c>
+      <c r="AC3" s="75">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>19.583333333333332</v>
-      </c>
-      <c r="AD3" s="77">
+        <v>58.75</v>
+      </c>
+      <c r="AD3" s="75">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>3.5</v>
-      </c>
-      <c r="AE3" s="75">
+        <v>10.5</v>
+      </c>
+      <c r="AE3" s="73">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="AF3" s="76">
+        <v>10</v>
+      </c>
+      <c r="AF3" s="74">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
         <v>0.25565087658475677</v>
       </c>
-      <c r="AG3" s="76">
+      <c r="AG3" s="74">
         <f>(('Reach Propertise'!$F3-'Reach Propertise'!$R3)/'Reach Propertise'!$F3)</f>
         <v>0.40352052448325898</v>
       </c>
-      <c r="AH3" s="76">
+      <c r="AH3" s="74">
         <f>((Table1[[#This Row],[Tt]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Tt]])</f>
         <v>0.81933273703513521</v>
       </c>
-      <c r="AI3" s="78">
+      <c r="AI3" s="76">
         <f>Table1[[#This Row],[width '[meters']]]/Table1[[#This Row],[depth '[meters']]]</f>
         <v>45.603754840751279</v>
       </c>
-      <c r="AJ3" s="75">
+      <c r="AJ3" s="73">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>406.6923060318</v>
-      </c>
-      <c r="AK3" s="75">
+        <v>135.56410201060001</v>
+      </c>
+      <c r="AK3" s="73">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
         <v>-0.56669999999999998</v>
       </c>
-      <c r="AL3" s="75">
+      <c r="AL3" s="73">
         <v>1</v>
       </c>
-      <c r="AM3" s="75">
+      <c r="AM3" s="73">
         <f>'Reach Propertise'!$F3</f>
         <v>0.43330000000000002</v>
       </c>
-      <c r="AN3" s="75">
+      <c r="AN3" s="73">
         <v>1</v>
       </c>
-      <c r="AO3" s="99">
+      <c r="AO3" s="97">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>19</v>
-      </c>
-      <c r="AP3" s="99">
+        <v>58</v>
+      </c>
+      <c r="AP3" s="97">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:42" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+    <row r="4" spans="1:42" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="78" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="71">
+      <c r="B4" s="69">
         <v>1175</v>
       </c>
-      <c r="C4" s="71">
+      <c r="C4" s="69">
         <v>2875</v>
       </c>
-      <c r="D4" s="71">
+      <c r="D4" s="69">
         <v>7.24</v>
       </c>
-      <c r="E4" s="71">
+      <c r="E4" s="69">
         <f>3.25*1000/3600</f>
         <v>0.90277777777777779</v>
       </c>
-      <c r="F4" s="71">
+      <c r="F4" s="69">
         <v>1.1333</v>
       </c>
-      <c r="G4" s="71">
+      <c r="G4" s="69">
         <f>8.8*1000/3600</f>
         <v>2.4444444444444446</v>
       </c>
-      <c r="H4" s="71">
+      <c r="H4" s="69">
         <v>7.24</v>
       </c>
-      <c r="I4" s="71"/>
-      <c r="J4" s="81">
+      <c r="I4" s="69"/>
+      <c r="J4" s="79">
         <f>11.76/10000</f>
         <v>1.176E-3</v>
       </c>
-      <c r="K4" s="81">
+      <c r="K4" s="79">
         <v>0.57269499999999995</v>
       </c>
-      <c r="L4" s="81">
+      <c r="L4" s="79">
         <v>16.589739999999999</v>
       </c>
-      <c r="M4" s="81">
+      <c r="M4" s="79">
         <v>0.11053590000000001</v>
       </c>
-      <c r="N4" s="75"/>
-      <c r="O4" s="75"/>
-      <c r="P4" s="75"/>
-      <c r="Q4" s="82">
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="80">
         <f>Table1[Q '[m3/sec']]/(Table1[depth '[meters']]*Table1[width '[meters']])</f>
         <v>0.76203618663908446</v>
       </c>
-      <c r="R4" s="75">
+      <c r="R4" s="73">
         <f>(Table1[[#This Row],[Reach Length '[meters']]]/(Table1[[#This Row],[Q '[m3/sec']]]/(Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]])))/3600</f>
         <v>0.61968477416398082</v>
       </c>
-      <c r="S4" s="75">
+      <c r="S4" s="73">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
         <v>0.70467758855652618</v>
       </c>
-      <c r="T4" s="75">
+      <c r="T4" s="73">
         <v>1</v>
       </c>
-      <c r="U4" s="75">
+      <c r="U4" s="73">
         <v>0</v>
       </c>
-      <c r="V4" s="75">
+      <c r="V4" s="73">
         <v>0</v>
       </c>
-      <c r="W4" s="83">
+      <c r="W4" s="81">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>2.875</v>
       </c>
-      <c r="X4" s="97">
+      <c r="X4" s="95">
         <v>0.11053590000000001</v>
       </c>
-      <c r="Y4" s="76" t="str">
+      <c r="Y4" s="74" t="str">
         <f>IF(AVERAGE(Table1[[#This Row],[Error Ti]]&lt;=AVERAGE(Table1[[#This Row],[Error Tp]])),"use Ti","use Tp")</f>
         <v>use Ti</v>
       </c>
-      <c r="Z4" s="75">
+      <c r="Z4" s="73">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]-Table1[[#This Row],[Start point distance '[meters']]]</f>
         <v>1700</v>
       </c>
-      <c r="AA4" s="83">
+      <c r="AA4" s="81">
         <f>(Table1[[#This Row],[Tp]]-AN4)*3600</f>
         <v>4079.88</v>
       </c>
-      <c r="AB4" s="84">
+      <c r="AB4" s="82">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>271</v>
-      </c>
-      <c r="AC4" s="84">
+        <v>407</v>
+      </c>
+      <c r="AC4" s="82">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>47.916666666666664</v>
-      </c>
-      <c r="AD4" s="84">
+        <v>143.75</v>
+      </c>
+      <c r="AD4" s="82">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>19.583333333333332</v>
-      </c>
-      <c r="AE4" s="75">
+        <v>58.75</v>
+      </c>
+      <c r="AE4" s="73">
         <f>Delta_T__seconds</f>
-        <v>15</v>
-      </c>
-      <c r="AF4" s="76">
+        <v>10</v>
+      </c>
+      <c r="AF4" s="74">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
         <v>0.31357994246451354</v>
       </c>
-      <c r="AG4" s="76">
+      <c r="AG4" s="74">
         <f>(('Reach Propertise'!$F4-'Reach Propertise'!$R4)/'Reach Propertise'!$F4)</f>
         <v>0.45320323465633033</v>
       </c>
-      <c r="AH4" s="76">
+      <c r="AH4" s="74">
         <f>((Table1[[#This Row],[Tt]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Tt]])</f>
         <v>0.74649259238746246</v>
       </c>
-      <c r="AI4" s="78">
+      <c r="AI4" s="76">
         <f>Table1[[#This Row],[width '[meters']]]/Table1[[#This Row],[depth '[meters']]]</f>
         <v>28.967845013488855</v>
       </c>
-      <c r="AJ4" s="83">
+      <c r="AJ4" s="81">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>570.05166895799994</v>
-      </c>
-      <c r="AK4" s="83">
+        <v>190.01722298599998</v>
+      </c>
+      <c r="AK4" s="81">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
         <v>1.1333</v>
       </c>
-      <c r="AL4" s="75"/>
-      <c r="AM4" s="75">
+      <c r="AL4" s="73"/>
+      <c r="AM4" s="73">
         <f>'Reach Propertise'!$F4</f>
         <v>1.1333</v>
       </c>
-      <c r="AN4" s="75"/>
-      <c r="AO4" s="99">
+      <c r="AN4" s="73"/>
+      <c r="AO4" s="97">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>47</v>
-      </c>
-      <c r="AP4" s="99">
+        <v>143</v>
+      </c>
+      <c r="AP4" s="97">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:42" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="80" t="s">
+    <row r="5" spans="1:42" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="71">
+      <c r="B5" s="69">
         <v>2875</v>
       </c>
-      <c r="C5" s="71">
+      <c r="C5" s="69">
         <v>5275</v>
       </c>
-      <c r="D5" s="71">
+      <c r="D5" s="69">
         <v>7.51</v>
       </c>
-      <c r="E5" s="71">
+      <c r="E5" s="69">
         <f>3.75*1000/3600</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="F5" s="71">
+      <c r="F5" s="69">
         <v>2.4666999999999999</v>
       </c>
-      <c r="G5" s="71">
+      <c r="G5" s="69">
         <f>14.8*1000/3600</f>
         <v>4.1111111111111107</v>
       </c>
-      <c r="H5" s="71">
+      <c r="H5" s="69">
         <v>7.51</v>
       </c>
-      <c r="I5" s="71"/>
-      <c r="J5" s="81">
+      <c r="I5" s="69"/>
+      <c r="J5" s="79">
         <f>16.67/10000</f>
         <v>1.6670000000000001E-3</v>
       </c>
-      <c r="K5" s="81">
+      <c r="K5" s="79">
         <v>0.62161200000000005</v>
       </c>
-      <c r="L5" s="81">
+      <c r="L5" s="79">
         <v>17.83409</v>
       </c>
-      <c r="M5" s="81">
+      <c r="M5" s="79">
         <v>5.8002699999999997E-2</v>
       </c>
-      <c r="N5" s="75"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="75"/>
-      <c r="Q5" s="82">
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="80">
         <f>Table1[Q '[m3/sec']]/(Table1[depth '[meters']]*Table1[width '[meters']])</f>
         <v>0.67743806094400494</v>
       </c>
-      <c r="R5" s="75">
+      <c r="R5" s="73">
         <f>(Table1[[#This Row],[Reach Length '[meters']]]/(Table1[[#This Row],[Q '[m3/sec']]]/(Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]])))/3600</f>
         <v>0.98409980941677766</v>
       </c>
-      <c r="S5" s="75">
+      <c r="S5" s="73">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
         <v>0.59402350418688044</v>
       </c>
-      <c r="T5" s="75">
+      <c r="T5" s="73">
         <v>1</v>
       </c>
-      <c r="U5" s="75">
+      <c r="U5" s="73">
         <v>0</v>
       </c>
-      <c r="V5" s="75">
+      <c r="V5" s="73">
         <v>0</v>
       </c>
-      <c r="W5" s="83">
+      <c r="W5" s="81">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>5.2750000000000004</v>
       </c>
-      <c r="X5" s="97">
+      <c r="X5" s="95">
         <v>5.8002699999999997E-2</v>
       </c>
-      <c r="Y5" s="76" t="str">
+      <c r="Y5" s="74" t="str">
         <f>IF(AVERAGE(Table1[[#This Row],[Error Ti]]&lt;=AVERAGE(Table1[[#This Row],[Error Tp]])),"use Ti","use Tp")</f>
         <v>use Ti</v>
       </c>
-      <c r="Z5" s="75">
+      <c r="Z5" s="73">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]-Table1[[#This Row],[Start point distance '[meters']]]</f>
         <v>2400</v>
       </c>
-      <c r="AA5" s="83">
+      <c r="AA5" s="81">
         <f>(Table1[[#This Row],[Tp]]-AN5)*3600</f>
         <v>8880.119999999999</v>
       </c>
-      <c r="AB5" s="84">
+      <c r="AB5" s="82">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>592</v>
-      </c>
-      <c r="AC5" s="84">
+        <v>888</v>
+      </c>
+      <c r="AC5" s="82">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>87.916666666666671</v>
-      </c>
-      <c r="AD5" s="84">
+        <v>263.75</v>
+      </c>
+      <c r="AD5" s="82">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>47.916666666666664</v>
-      </c>
-      <c r="AE5" s="75">
+        <v>143.75</v>
+      </c>
+      <c r="AE5" s="73">
         <f>Delta_T__seconds</f>
-        <v>15</v>
-      </c>
-      <c r="AF5" s="76">
+        <v>10</v>
+      </c>
+      <c r="AF5" s="74">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
         <v>5.5264182959893514E-2</v>
       </c>
-      <c r="AG5" s="76">
+      <c r="AG5" s="74">
         <f>(('Reach Propertise'!$F5-'Reach Propertise'!$R5)/'Reach Propertise'!$F5)</f>
         <v>0.60104600907415673</v>
       </c>
-      <c r="AH5" s="76">
+      <c r="AH5" s="74">
         <f>((Table1[[#This Row],[Tt]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Tt]])</f>
         <v>0.7606243706824054</v>
       </c>
-      <c r="AI5" s="78">
+      <c r="AI5" s="76">
         <f>Table1[[#This Row],[width '[meters']]]/Table1[[#This Row],[depth '[meters']]]</f>
         <v>28.690067115821442</v>
       </c>
-      <c r="AJ5" s="83">
+      <c r="AJ5" s="81">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>665.15306118480009</v>
-      </c>
-      <c r="AK5" s="83">
+        <v>221.71768706160003</v>
+      </c>
+      <c r="AK5" s="81">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
         <v>2.4666999999999999</v>
       </c>
-      <c r="AL5" s="75"/>
-      <c r="AM5" s="75">
+      <c r="AL5" s="73"/>
+      <c r="AM5" s="73">
         <f>'Reach Propertise'!$F5</f>
         <v>2.4666999999999999</v>
       </c>
-      <c r="AN5" s="75"/>
-      <c r="AO5" s="99">
+      <c r="AN5" s="73"/>
+      <c r="AO5" s="97">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>87</v>
-      </c>
-      <c r="AP5" s="99">
+        <v>263</v>
+      </c>
+      <c r="AP5" s="97">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:42" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="80" t="s">
+    <row r="6" spans="1:42" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="71">
+      <c r="B6" s="69">
         <v>5275</v>
       </c>
-      <c r="C6" s="71">
+      <c r="C6" s="69">
         <v>7775</v>
       </c>
-      <c r="D6" s="71">
+      <c r="D6" s="69">
         <v>9.25</v>
       </c>
-      <c r="E6" s="71">
+      <c r="E6" s="69">
         <f>10.5*1000/3600</f>
         <v>2.9166666666666665</v>
       </c>
-      <c r="F6" s="71">
+      <c r="F6" s="69">
         <v>3.7332999999999998</v>
       </c>
-      <c r="G6" s="71">
+      <c r="G6" s="69">
         <f>20*1000/3600</f>
         <v>5.5555555555555554</v>
       </c>
-      <c r="H6" s="71">
+      <c r="H6" s="69">
         <v>9.25</v>
       </c>
-      <c r="I6" s="71"/>
-      <c r="J6" s="81">
+      <c r="I6" s="69"/>
+      <c r="J6" s="79">
         <f>24/10000</f>
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="K6" s="81">
+      <c r="K6" s="79">
         <v>0.52793800000000002</v>
       </c>
-      <c r="L6" s="81">
+      <c r="L6" s="79">
         <v>34.910490000000003</v>
       </c>
-      <c r="M6" s="81">
+      <c r="M6" s="79">
         <v>3.4605400000000001E-2</v>
       </c>
-      <c r="N6" s="75"/>
-      <c r="O6" s="75"/>
-      <c r="P6" s="75"/>
-      <c r="Q6" s="82">
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="80">
         <f>Table1[Q '[m3/sec']]/(Table1[depth '[meters']]*Table1[width '[meters']])</f>
         <v>0.50188343915290901</v>
       </c>
-      <c r="R6" s="75">
+      <c r="R6" s="73">
         <f>(Table1[[#This Row],[Reach Length '[meters']]]/(Table1[[#This Row],[Q '[m3/sec']]]/(Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]])))/3600</f>
         <v>1.3836767469684685</v>
       </c>
-      <c r="S6" s="75">
+      <c r="S6" s="73">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
         <v>0.57850218900763994</v>
       </c>
-      <c r="T6" s="75">
+      <c r="T6" s="73">
         <v>1</v>
       </c>
-      <c r="U6" s="75">
+      <c r="U6" s="73">
         <v>0</v>
       </c>
-      <c r="V6" s="75">
+      <c r="V6" s="73">
         <v>0</v>
       </c>
-      <c r="W6" s="83">
+      <c r="W6" s="81">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>7.7750000000000004</v>
       </c>
-      <c r="X6" s="97">
+      <c r="X6" s="95">
         <v>3.4605400000000001E-2</v>
       </c>
-      <c r="Y6" s="76" t="str">
+      <c r="Y6" s="74" t="str">
         <f>IF(AVERAGE(Table1[[#This Row],[Error Ti]]&lt;=AVERAGE(Table1[[#This Row],[Error Tp]])),"use Ti","use Tp")</f>
         <v>use Ti</v>
       </c>
-      <c r="Z6" s="75">
+      <c r="Z6" s="73">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]-Table1[[#This Row],[Start point distance '[meters']]]</f>
         <v>2500</v>
       </c>
-      <c r="AA6" s="83">
+      <c r="AA6" s="81">
         <f>(Table1[[#This Row],[Tp]]-AN6)*3600</f>
         <v>13439.88</v>
       </c>
-      <c r="AB6" s="84">
+      <c r="AB6" s="82">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>895</v>
-      </c>
-      <c r="AC6" s="84">
+        <v>1343</v>
+      </c>
+      <c r="AC6" s="82">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>129.58333333333334</v>
-      </c>
-      <c r="AD6" s="84">
+        <v>388.75</v>
+      </c>
+      <c r="AD6" s="82">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>87.916666666666671</v>
-      </c>
-      <c r="AE6" s="75">
+        <v>263.75</v>
+      </c>
+      <c r="AE6" s="73">
         <f>Delta_T__seconds</f>
-        <v>15</v>
-      </c>
-      <c r="AF6" s="76">
+        <v>10</v>
+      </c>
+      <c r="AF6" s="74">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
         <v>0.52559654389652499</v>
       </c>
-      <c r="AG6" s="76">
+      <c r="AG6" s="74">
         <f>(('Reach Propertise'!$F6-'Reach Propertise'!$R6)/'Reach Propertise'!$F6)</f>
         <v>0.6293689907137201</v>
       </c>
-      <c r="AH6" s="76">
+      <c r="AH6" s="74">
         <f>((Table1[[#This Row],[Tt]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Tt]])</f>
         <v>0.7509381855456756</v>
       </c>
-      <c r="AI6" s="78">
+      <c r="AI6" s="76">
         <f>Table1[[#This Row],[width '[meters']]]/Table1[[#This Row],[depth '[meters']]]</f>
         <v>66.126117081930076</v>
       </c>
-      <c r="AJ6" s="83">
+      <c r="AJ6" s="81">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>1105.8344561772001</v>
-      </c>
-      <c r="AK6" s="83">
+        <v>368.61148539240003</v>
+      </c>
+      <c r="AK6" s="81">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
         <v>3.7332999999999998</v>
       </c>
-      <c r="AL6" s="75"/>
-      <c r="AM6" s="75">
+      <c r="AL6" s="73"/>
+      <c r="AM6" s="73">
         <f>'Reach Propertise'!$F6</f>
         <v>3.7332999999999998</v>
       </c>
-      <c r="AN6" s="75"/>
-      <c r="AO6" s="99">
+      <c r="AN6" s="73"/>
+      <c r="AO6" s="97">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>129</v>
-      </c>
-      <c r="AP6" s="99">
+        <v>388</v>
+      </c>
+      <c r="AP6" s="97">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:42" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="80" t="s">
+    <row r="7" spans="1:42" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="71">
+      <c r="B7" s="69">
         <v>7775</v>
       </c>
-      <c r="C7" s="71">
+      <c r="C7" s="69">
         <v>10275</v>
       </c>
-      <c r="D7" s="71">
+      <c r="D7" s="69">
         <v>9.8000000000000007</v>
       </c>
-      <c r="E7" s="71">
+      <c r="E7" s="69">
         <f>15.1*1000/3600</f>
         <v>4.1944444444444446</v>
       </c>
-      <c r="F7" s="71">
+      <c r="F7" s="69">
         <v>5.0332999999999997</v>
       </c>
-      <c r="G7" s="71">
+      <c r="G7" s="69">
         <f>26*1000/3600</f>
         <v>7.2222222222222223</v>
       </c>
-      <c r="H7" s="71">
+      <c r="H7" s="69">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I7" s="71"/>
-      <c r="J7" s="81">
+      <c r="I7" s="69"/>
+      <c r="J7" s="79">
         <f>44/10000</f>
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="K7" s="81">
+      <c r="K7" s="79">
         <v>0.42355799999999999</v>
       </c>
-      <c r="L7" s="81">
+      <c r="L7" s="79">
         <v>31.004169999999998</v>
       </c>
-      <c r="M7" s="81">
+      <c r="M7" s="79">
         <v>2.1080000000000002E-2</v>
       </c>
-      <c r="N7" s="75"/>
-      <c r="O7" s="75"/>
-      <c r="P7" s="75"/>
-      <c r="Q7" s="82">
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="80">
         <f>Table1[Q '[m3/sec']]/(Table1[depth '[meters']]*Table1[width '[meters']])</f>
         <v>0.74626500626555514</v>
       </c>
-      <c r="R7" s="75">
+      <c r="R7" s="73">
         <f>(Table1[[#This Row],[Reach Length '[meters']]]/(Table1[[#This Row],[Q '[m3/sec']]]/(Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]])))/3600</f>
         <v>0.93056010748724483</v>
       </c>
-      <c r="S7" s="75">
+      <c r="S7" s="73">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
         <v>0.56705673547506941</v>
       </c>
-      <c r="T7" s="75">
+      <c r="T7" s="73">
         <v>1</v>
       </c>
-      <c r="U7" s="75">
+      <c r="U7" s="73">
         <v>0</v>
       </c>
-      <c r="V7" s="75">
+      <c r="V7" s="73">
         <v>0</v>
       </c>
-      <c r="W7" s="83">
+      <c r="W7" s="81">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>10.275</v>
       </c>
-      <c r="X7" s="97">
+      <c r="X7" s="95">
         <v>2.1080000000000002E-2</v>
       </c>
-      <c r="Y7" s="76" t="str">
+      <c r="Y7" s="74" t="str">
         <f>IF(AVERAGE(Table1[[#This Row],[Error Ti]]&lt;=AVERAGE(Table1[[#This Row],[Error Tp]])),"use Ti","use Tp")</f>
         <v>use Ti</v>
       </c>
-      <c r="Z7" s="75">
+      <c r="Z7" s="73">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]-Table1[[#This Row],[Start point distance '[meters']]]</f>
         <v>2500</v>
       </c>
-      <c r="AA7" s="83">
+      <c r="AA7" s="81">
         <f>(Table1[[#This Row],[Tp]]-AN7)*3600</f>
         <v>18119.879999999997</v>
       </c>
-      <c r="AB7" s="84">
+      <c r="AB7" s="82">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>1207</v>
-      </c>
-      <c r="AC7" s="84">
+        <v>1811</v>
+      </c>
+      <c r="AC7" s="82">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>171.25</v>
-      </c>
-      <c r="AD7" s="84">
+        <v>513.75</v>
+      </c>
+      <c r="AD7" s="82">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>129.58333333333334</v>
-      </c>
-      <c r="AE7" s="75">
+        <v>388.75</v>
+      </c>
+      <c r="AE7" s="73">
         <f>Delta_T__seconds</f>
-        <v>15</v>
-      </c>
-      <c r="AF7" s="76">
+        <v>10</v>
+      </c>
+      <c r="AF7" s="74">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
         <v>0.7781446101354913</v>
       </c>
-      <c r="AG7" s="76">
+      <c r="AG7" s="74">
         <f>(('Reach Propertise'!$F7-'Reach Propertise'!$R7)/'Reach Propertise'!$F7)</f>
         <v>0.8151192840706406</v>
       </c>
-      <c r="AH7" s="76">
+      <c r="AH7" s="74">
         <f>((Table1[[#This Row],[Tt]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Tt]])</f>
         <v>0.8711532158863815</v>
       </c>
-      <c r="AI7" s="78">
+      <c r="AI7" s="76">
         <f>Table1[[#This Row],[width '[meters']]]/Table1[[#This Row],[depth '[meters']]]</f>
         <v>73.199349321698563</v>
       </c>
-      <c r="AJ7" s="83">
+      <c r="AJ7" s="81">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>787.92385421159997</v>
-      </c>
-      <c r="AK7" s="83">
+        <v>262.64128473720001</v>
+      </c>
+      <c r="AK7" s="81">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
         <v>5.0332999999999997</v>
       </c>
-      <c r="AL7" s="75"/>
-      <c r="AM7" s="75">
+      <c r="AL7" s="73"/>
+      <c r="AM7" s="73">
         <f>'Reach Propertise'!$F7</f>
         <v>5.0332999999999997</v>
       </c>
-      <c r="AN7" s="75"/>
-      <c r="AO7" s="99">
+      <c r="AN7" s="73"/>
+      <c r="AO7" s="97">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>171</v>
-      </c>
-      <c r="AP7" s="99">
+        <v>513</v>
+      </c>
+      <c r="AP7" s="97">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:42" s="79" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="80" t="s">
+    <row r="8" spans="1:42" s="77" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="78" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="71">
+      <c r="B8" s="69">
         <v>10275</v>
       </c>
-      <c r="C8" s="71">
+      <c r="C8" s="69">
         <v>13775</v>
       </c>
-      <c r="D8" s="71">
+      <c r="D8" s="69">
         <v>10</v>
       </c>
-      <c r="E8" s="71">
+      <c r="E8" s="69">
         <f>19*1000/3600</f>
         <v>5.2777777777777777</v>
       </c>
-      <c r="F8" s="71">
+      <c r="F8" s="69">
         <v>6.5369000000000002</v>
       </c>
-      <c r="G8" s="71">
+      <c r="G8" s="69">
         <f>33.5*1000/3600</f>
         <v>9.3055555555555554</v>
       </c>
-      <c r="H8" s="71">
+      <c r="H8" s="69">
         <v>10</v>
       </c>
-      <c r="I8" s="71"/>
-      <c r="J8" s="81">
+      <c r="I8" s="69"/>
+      <c r="J8" s="79">
         <f>25.71/10000</f>
         <v>2.5709999999999999E-3</v>
       </c>
-      <c r="K8" s="81">
+      <c r="K8" s="79">
         <v>0.62438099999999996</v>
       </c>
-      <c r="L8" s="81">
+      <c r="L8" s="79">
         <v>23.586819999999999</v>
       </c>
-      <c r="M8" s="81">
+      <c r="M8" s="79">
         <v>2.0655E-2</v>
       </c>
-      <c r="N8" s="75"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="75"/>
-      <c r="Q8" s="82">
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="80">
         <f>Table1[Q '[m3/sec']]/(Table1[depth '[meters']]*Table1[width '[meters']])</f>
         <v>0.67901743896945754</v>
       </c>
-      <c r="R8" s="75">
+      <c r="R8" s="73">
         <f>(Table1[[#This Row],[Reach Length '[meters']]]/(Table1[[#This Row],[Q '[m3/sec']]]/(Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]])))/3600</f>
         <v>1.4318074417908333</v>
       </c>
-      <c r="S8" s="75">
+      <c r="S8" s="73">
         <f>(Table1[[#This Row],[End Point distance  '[meters']]]/(3600*Table1[[#This Row],[Tp]]))</f>
         <v>0.58535221418239358</v>
       </c>
-      <c r="T8" s="75">
+      <c r="T8" s="73">
         <v>1</v>
       </c>
-      <c r="U8" s="75">
+      <c r="U8" s="73">
         <v>0</v>
       </c>
-      <c r="V8" s="75">
+      <c r="V8" s="73">
         <v>0</v>
       </c>
-      <c r="W8" s="83">
+      <c r="W8" s="81">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/1000</f>
         <v>13.775</v>
       </c>
-      <c r="X8" s="97">
+      <c r="X8" s="95">
         <v>2.0655E-2</v>
       </c>
-      <c r="Y8" s="76" t="str">
+      <c r="Y8" s="74" t="str">
         <f>IF(AVERAGE(Table1[[#This Row],[Error Ti]]&lt;=AVERAGE(Table1[[#This Row],[Error Tp]])),"use Ti","use Tp")</f>
         <v>use Ti</v>
       </c>
-      <c r="Z8" s="75">
+      <c r="Z8" s="73">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]-Table1[[#This Row],[Start point distance '[meters']]]</f>
         <v>3500</v>
       </c>
-      <c r="AA8" s="83">
+      <c r="AA8" s="81">
         <f>(Table1[[#This Row],[Tp]]-AN8)*3600</f>
         <v>23532.84</v>
       </c>
-      <c r="AB8" s="84">
+      <c r="AB8" s="82">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>1568</v>
-      </c>
-      <c r="AC8" s="84">
+        <v>2353</v>
+      </c>
+      <c r="AC8" s="82">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
-        <v>229.58333333333334</v>
-      </c>
-      <c r="AD8" s="84">
+        <v>688.75</v>
+      </c>
+      <c r="AD8" s="82">
         <f>Table1[[#This Row],[Start point distance '[meters']]]/Delta_X__meters</f>
-        <v>171.25</v>
-      </c>
-      <c r="AE8" s="75">
+        <v>513.75</v>
+      </c>
+      <c r="AE8" s="73">
         <f>Delta_T__seconds</f>
-        <v>15</v>
-      </c>
-      <c r="AF8" s="76">
+        <v>10</v>
+      </c>
+      <c r="AF8" s="74">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
         <v>0.72871016892384211</v>
       </c>
-      <c r="AG8" s="76">
+      <c r="AG8" s="74">
         <f>(('Reach Propertise'!$F8-'Reach Propertise'!$R8)/'Reach Propertise'!$F8)</f>
         <v>0.78096537475090133</v>
       </c>
-      <c r="AH8" s="76">
+      <c r="AH8" s="74">
         <f>((Table1[[#This Row],[Tt]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Tt]])</f>
         <v>0.84613412565829849</v>
       </c>
-      <c r="AI8" s="78">
+      <c r="AI8" s="76">
         <f>Table1[[#This Row],[width '[meters']]]/Table1[[#This Row],[depth '[meters']]]</f>
         <v>37.776325672946484</v>
       </c>
-      <c r="AJ8" s="83">
+      <c r="AJ8" s="81">
         <f>Table1[[#This Row],[depth '[meters']]]*Table1[[#This Row],[width '[meters']]]*Delta_X__meters</f>
-        <v>883.62973550519985</v>
-      </c>
-      <c r="AK8" s="83">
+        <v>294.54324516839995</v>
+      </c>
+      <c r="AK8" s="81">
         <f>Table1[[#This Row],[Column3]]-Table1[[#This Row],[Column2]]</f>
         <v>6.5369000000000002</v>
       </c>
-      <c r="AL8" s="75"/>
-      <c r="AM8" s="75">
+      <c r="AL8" s="73"/>
+      <c r="AM8" s="73">
         <f>'Reach Propertise'!$F8</f>
         <v>6.5369000000000002</v>
       </c>
-      <c r="AN8" s="75"/>
-      <c r="AO8" s="99">
+      <c r="AN8" s="73"/>
+      <c r="AO8" s="97">
         <f>FLOOR(Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters,1)</f>
-        <v>229</v>
-      </c>
-      <c r="AP8" s="99">
+        <v>688</v>
+      </c>
+      <c r="AP8" s="97">
         <f>((1/1000000)*Table1[[#This Row],[Cup]]*Table1[[#This Row],[R ratio]]*Table1[[#This Row],[Inj Mass]])/Table1[[#This Row],[Q '[m3/sec']]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:42" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="X9" s="86"/>
-      <c r="Y9" s="87"/>
-    </row>
-    <row r="10" spans="1:42" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="X10" s="86"/>
-      <c r="Y10" s="87"/>
-    </row>
-    <row r="11" spans="1:42" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="X11" s="68"/>
-      <c r="Y11" s="69"/>
+    <row r="9" spans="1:42" s="83" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X9" s="84"/>
+      <c r="Y9" s="85"/>
+    </row>
+    <row r="10" spans="1:42" s="83" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X10" s="84"/>
+      <c r="Y10" s="85"/>
+    </row>
+    <row r="11" spans="1:42" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X11" s="66"/>
+      <c r="Y11" s="67"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8280,41 +8291,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="56" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="57"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8349,80 +8360,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="22" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="59" t="s">
+      <c r="G1" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="59" t="s">
+      <c r="H1" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="57" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="60">
-        <v>1100</v>
+      <c r="A2" s="58">
+        <v>25</v>
       </c>
       <c r="B2" s="13">
         <v>1000</v>
       </c>
-      <c r="C2" s="61">
+      <c r="C2" s="59">
         <v>0</v>
       </c>
-      <c r="D2" s="60">
+      <c r="D2" s="58">
         <v>25</v>
       </c>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
       <c r="M2" s="24"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I4" s="24"/>
@@ -8439,7 +8450,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="P2" sqref="P2:P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8463,8 +8474,8 @@
       <c r="H2">
         <v>5</v>
       </c>
-      <c r="P2" s="89" t="s">
-        <v>112</v>
+      <c r="P2" s="87" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8474,7 +8485,7 @@
       <c r="H3">
         <v>10</v>
       </c>
-      <c r="P3" s="90" t="s">
+      <c r="P3" s="88" t="s">
         <v>85</v>
       </c>
     </row>
@@ -8485,7 +8496,7 @@
       <c r="H4">
         <v>25</v>
       </c>
-      <c r="P4" s="90" t="s">
+      <c r="P4" s="88" t="s">
         <v>86</v>
       </c>
     </row>
@@ -8496,7 +8507,7 @@
       <c r="H5">
         <v>50</v>
       </c>
-      <c r="P5" s="90" t="s">
+      <c r="P5" s="88" t="s">
         <v>87</v>
       </c>
     </row>
@@ -8507,7 +8518,7 @@
       <c r="H6">
         <v>100</v>
       </c>
-      <c r="P6" s="90" t="s">
+      <c r="P6" s="88" t="s">
         <v>88</v>
       </c>
     </row>
@@ -8518,7 +8529,7 @@
       <c r="H7">
         <v>150</v>
       </c>
-      <c r="P7" s="90" t="s">
+      <c r="P7" s="88" t="s">
         <v>89</v>
       </c>
     </row>
@@ -8529,7 +8540,7 @@
       <c r="H8">
         <v>200</v>
       </c>
-      <c r="P8" s="90" t="s">
+      <c r="P8" s="88" t="s">
         <v>90</v>
       </c>
     </row>
@@ -8540,7 +8551,7 @@
       <c r="H9">
         <v>250</v>
       </c>
-      <c r="P9" s="90" t="s">
+      <c r="P9" s="88" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8551,7 +8562,7 @@
       <c r="H10">
         <v>300</v>
       </c>
-      <c r="P10" s="90" t="s">
+      <c r="P10" s="88" t="s">
         <v>92</v>
       </c>
     </row>
@@ -8559,31 +8570,31 @@
       <c r="H11">
         <v>350</v>
       </c>
-      <c r="P11" s="90" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P11" s="88" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H12">
         <v>400</v>
       </c>
-      <c r="P12" s="91" t="s">
-        <v>110</v>
+      <c r="P12" s="89" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H13">
         <v>450</v>
       </c>
-      <c r="P13" s="90" t="s">
-        <v>94</v>
+      <c r="P13" s="88" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H14">
         <v>500</v>
       </c>
-      <c r="P14" s="90" t="s">
+      <c r="P14" s="88" t="s">
         <v>95</v>
       </c>
     </row>
@@ -8591,7 +8602,7 @@
       <c r="H15">
         <v>550</v>
       </c>
-      <c r="P15" s="90" t="s">
+      <c r="P15" s="88" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8599,7 +8610,7 @@
       <c r="H16">
         <v>600</v>
       </c>
-      <c r="P16" s="90" t="s">
+      <c r="P16" s="88" t="s">
         <v>97</v>
       </c>
     </row>
@@ -8607,7 +8618,7 @@
       <c r="H17">
         <v>650</v>
       </c>
-      <c r="P17" s="90" t="s">
+      <c r="P17" s="88" t="s">
         <v>98</v>
       </c>
     </row>
@@ -8615,7 +8626,7 @@
       <c r="H18">
         <v>700</v>
       </c>
-      <c r="P18" s="90" t="s">
+      <c r="P18" s="88" t="s">
         <v>99</v>
       </c>
     </row>
@@ -8623,7 +8634,7 @@
       <c r="H19">
         <v>750</v>
       </c>
-      <c r="P19" s="90" t="s">
+      <c r="P19" s="88" t="s">
         <v>100</v>
       </c>
     </row>
@@ -8631,40 +8642,40 @@
       <c r="H20">
         <v>800</v>
       </c>
-      <c r="P20" s="90" t="s">
-        <v>101</v>
+      <c r="P20" s="88" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="8:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H21">
         <v>900</v>
       </c>
-      <c r="P21" s="90" t="s">
-        <v>102</v>
+      <c r="P21" s="88" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H22">
         <v>1000</v>
       </c>
-      <c r="P22" s="92" t="s">
-        <v>111</v>
+      <c r="P22" s="90" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>1250</v>
       </c>
-      <c r="P23" s="92"/>
+      <c r="P23" s="90"/>
     </row>
     <row r="24" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H24">
         <v>1500</v>
       </c>
-      <c r="P24" s="93"/>
+      <c r="P24" s="91"/>
     </row>
     <row r="25" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="P25" s="94"/>
+      <c r="P25" s="92"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8694,10 +8705,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X26"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8723,66 +8734,66 @@
     <col min="19" max="19" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="100" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+    <row r="1" spans="1:19" s="98" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="98" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="98" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="100" t="s">
+      <c r="C1" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="100" t="s">
+      <c r="E1" s="98" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="100" t="s">
+      <c r="G1" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="100" t="s">
+      <c r="H1" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="100" t="s">
+      <c r="I1" s="98" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="100" t="s">
-        <v>116</v>
-      </c>
-      <c r="K1" s="100" t="s">
+      <c r="J1" s="98" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="98" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="100" t="s">
+      <c r="L1" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="100" t="s">
+      <c r="M1" s="98" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="100" t="s">
+      <c r="N1" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="100" t="s">
+      <c r="O1" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="P1" s="100" t="s">
+      <c r="P1" s="98" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="100" t="s">
+      <c r="Q1" s="98" t="s">
         <v>100</v>
       </c>
-      <c r="R1" s="100" t="s">
+      <c r="R1" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="S1" s="100" t="s">
+      <c r="S1" s="98" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.68015664268852827</v>
       </c>
@@ -8841,7 +8852,7 @@
         <v>13.942155495606716</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.31322849740396147</v>
       </c>
@@ -8900,7 +8911,7 @@
         <v>16.388113959583489</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.26698111766955995</v>
       </c>
@@ -8959,7 +8970,7 @@
         <v>15.377687775050815</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.35933783316164253</v>
       </c>
@@ -8993,7 +9004,7 @@
       <c r="K5">
         <v>35.177546386489475</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5">
         <v>28.096184267128709</v>
       </c>
       <c r="M5">
@@ -9018,7 +9029,7 @@
         <v>13.278955923320112</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.34387364708602081</v>
       </c>
@@ -9064,25 +9075,20 @@
       <c r="O6">
         <v>18.279787512399285</v>
       </c>
-      <c r="P6" s="38">
+      <c r="P6">
         <v>43.34296430768245</v>
       </c>
-      <c r="Q6" s="38">
+      <c r="Q6">
         <v>7.3080205694117195</v>
       </c>
-      <c r="R6" s="38">
+      <c r="R6">
         <v>33.465758842333642</v>
       </c>
-      <c r="S6" s="38">
+      <c r="S6">
         <v>24.85729790564373</v>
       </c>
-      <c r="T6" s="38"/>
-      <c r="U6" s="38"/>
-      <c r="V6" s="38"/>
-      <c r="W6" s="38"/>
-      <c r="X6" s="38"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.33506683054146424</v>
       </c>
@@ -9128,25 +9134,20 @@
       <c r="O7">
         <v>1.3901698702784904</v>
       </c>
-      <c r="P7" s="38">
+      <c r="P7">
         <v>37.450196851082339</v>
       </c>
-      <c r="Q7" s="38">
+      <c r="Q7">
         <v>7.4357658243047737</v>
       </c>
-      <c r="R7" s="38">
+      <c r="R7">
         <v>27.08994181247148</v>
       </c>
-      <c r="S7" s="38">
+      <c r="S7">
         <v>21.067085368232753</v>
       </c>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
-      <c r="V7" s="38"/>
-      <c r="W7" s="38"/>
-      <c r="X7" s="38"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.45280611092443795</v>
       </c>
@@ -9192,25 +9193,20 @@
       <c r="O8">
         <v>-6.9202824218865526</v>
       </c>
-      <c r="P8" s="38">
+      <c r="P8">
         <v>37.394201405106315</v>
       </c>
-      <c r="Q8" s="38">
+      <c r="Q8">
         <v>6.422533260982461</v>
       </c>
-      <c r="R8" s="38">
+      <c r="R8">
         <v>28.194582095621172</v>
       </c>
-      <c r="S8" s="38">
+      <c r="S8">
         <v>16.791435597158287</v>
       </c>
-      <c r="T8" s="38"/>
-      <c r="U8" s="38"/>
-      <c r="V8" s="38"/>
-      <c r="W8" s="38"/>
-      <c r="X8" s="38"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="e">
         <v>#N/A</v>
       </c>
@@ -9268,263 +9264,6 @@
       <c r="S9" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T9" s="38"/>
-      <c r="U9" s="38"/>
-      <c r="V9" s="38"/>
-      <c r="W9" s="38"/>
-      <c r="X9" s="38"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
-      <c r="U10" s="38"/>
-      <c r="V10" s="38"/>
-      <c r="W10" s="38"/>
-      <c r="X10" s="38"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="38"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
-      <c r="U12" s="38"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="38"/>
-      <c r="X12" s="38"/>
-    </row>
-    <row r="13" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="C13" s="100" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="100" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" s="100" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="100" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" s="100" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>0.68015664268852827</v>
-      </c>
-      <c r="D14">
-        <v>28625.050200190482</v>
-      </c>
-      <c r="E14">
-        <v>8397713719.6893826</v>
-      </c>
-      <c r="F14">
-        <v>16659637699.36138</v>
-      </c>
-      <c r="G14">
-        <v>5.4214850129549559</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>0.31322849740396147</v>
-      </c>
-      <c r="D15">
-        <v>68852.677170974173</v>
-      </c>
-      <c r="E15">
-        <v>1191998690413.3914</v>
-      </c>
-      <c r="F15">
-        <v>1694556080269.5063</v>
-      </c>
-      <c r="G15">
-        <v>10.147704164784699</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>0.26698111766955995</v>
-      </c>
-      <c r="D16">
-        <v>39274.013348111286</v>
-      </c>
-      <c r="E16">
-        <v>12738920.171506403</v>
-      </c>
-      <c r="F16">
-        <v>14182975.825430201</v>
-      </c>
-      <c r="G16">
-        <v>65535</v>
-      </c>
-    </row>
-    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <v>0.35933783316164253</v>
-      </c>
-      <c r="D17">
-        <v>64026.44107621452</v>
-      </c>
-      <c r="E17">
-        <v>11660815.389813524</v>
-      </c>
-      <c r="F17">
-        <v>15746001.233835166</v>
-      </c>
-      <c r="G17">
-        <v>149551654.81536677</v>
-      </c>
-    </row>
-    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <v>0.34387364708602081</v>
-      </c>
-      <c r="D18">
-        <v>9147441664.3559856</v>
-      </c>
-      <c r="E18">
-        <v>1.9290048029375352E+18</v>
-      </c>
-      <c r="F18">
-        <v>2.801819736520597E+18</v>
-      </c>
-      <c r="G18">
-        <v>18.279787512399285</v>
-      </c>
-      <c r="N18" s="38"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="38"/>
-      <c r="S18" s="38"/>
-      <c r="T18" s="38"/>
-    </row>
-    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <v>0.33506683054146424</v>
-      </c>
-      <c r="D19">
-        <v>621158150.54461765</v>
-      </c>
-      <c r="E19">
-        <v>2.2739472572257246E+20</v>
-      </c>
-      <c r="F19">
-        <v>3.6764427167066312E+20</v>
-      </c>
-      <c r="G19">
-        <v>1.3901698702784904</v>
-      </c>
-      <c r="M19" s="34"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-    </row>
-    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>0.45280611092443795</v>
-      </c>
-      <c r="D20">
-        <v>2723227.9512344319</v>
-      </c>
-      <c r="E20">
-        <v>7078511204.2171917</v>
-      </c>
-      <c r="F20">
-        <v>10784896704.219383</v>
-      </c>
-      <c r="G20">
-        <v>6.92028242188655</v>
-      </c>
-      <c r="M20" s="34"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="38"/>
-    </row>
-    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="M21" s="34"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="38"/>
-      <c r="Q21" s="38"/>
-      <c r="R21" s="38"/>
-      <c r="S21" s="38"/>
-      <c r="T21" s="38"/>
-    </row>
-    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="M22" s="34"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="38"/>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="38"/>
-      <c r="R22" s="38"/>
-      <c r="S22" s="38"/>
-      <c r="T22" s="38"/>
-    </row>
-    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="M23" s="34"/>
-      <c r="N23" s="38"/>
-      <c r="O23" s="38"/>
-      <c r="P23" s="38"/>
-      <c r="Q23" s="38"/>
-      <c r="R23" s="38"/>
-      <c r="S23" s="38"/>
-      <c r="T23" s="38"/>
-    </row>
-    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="M24" s="34"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="38"/>
-    </row>
-    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="M25" s="35"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="38"/>
-    </row>
-    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="M26" s="34"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="38"/>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
-      <c r="R26" s="38"/>
-      <c r="S26" s="38"/>
-      <c r="T26" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9549,30 +9288,30 @@
       <c r="K5" t="s">
         <v>80</v>
       </c>
-      <c r="L5" s="36">
+      <c r="L5" s="35">
         <v>16000</v>
       </c>
-      <c r="M5" s="36">
+      <c r="M5" s="35">
         <v>27900</v>
       </c>
-      <c r="N5" s="36">
+      <c r="N5" s="35">
         <v>36500</v>
       </c>
-      <c r="O5" s="36">
+      <c r="O5" s="35">
         <v>49600</v>
       </c>
-      <c r="P5" s="36">
+      <c r="P5" s="35">
         <v>57100</v>
       </c>
-      <c r="Q5" s="36">
+      <c r="Q5" s="35">
         <v>60000</v>
       </c>
-      <c r="R5" s="37">
+      <c r="R5" s="36">
         <v>76600</v>
       </c>
     </row>
     <row r="6" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K6" s="33" t="s">
+      <c r="K6" s="32" t="s">
         <v>75</v>
       </c>
       <c r="L6">
@@ -9598,7 +9337,7 @@
       </c>
     </row>
     <row r="7" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K7" s="34" t="s">
+      <c r="K7" s="33" t="s">
         <v>61</v>
       </c>
       <c r="L7">
@@ -9624,7 +9363,7 @@
       </c>
     </row>
     <row r="8" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="33" t="s">
         <v>66</v>
       </c>
       <c r="L8">
@@ -9650,7 +9389,7 @@
       </c>
     </row>
     <row r="9" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K9" s="34" t="s">
+      <c r="K9" s="33" t="s">
         <v>62</v>
       </c>
       <c r="L9">
@@ -9676,7 +9415,7 @@
       </c>
     </row>
     <row r="10" spans="11:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K10" s="34" t="s">
+      <c r="K10" s="33" t="s">
         <v>63</v>
       </c>
       <c r="L10">
@@ -9702,7 +9441,7 @@
       </c>
     </row>
     <row r="11" spans="11:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K11" s="34" t="s">
+      <c r="K11" s="33" t="s">
         <v>64</v>
       </c>
       <c r="L11">
@@ -9728,7 +9467,7 @@
       </c>
     </row>
     <row r="12" spans="11:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K12" s="34" t="s">
+      <c r="K12" s="33" t="s">
         <v>65</v>
       </c>
       <c r="L12">
@@ -9754,7 +9493,7 @@
       </c>
     </row>
     <row r="13" spans="11:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K13" s="35" t="s">
+      <c r="K13" s="34" t="s">
         <v>67</v>
       </c>
       <c r="L13">
@@ -9780,7 +9519,7 @@
       </c>
     </row>
     <row r="14" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K14" s="34" t="s">
+      <c r="K14" s="33" t="s">
         <v>68</v>
       </c>
       <c r="L14">
@@ -9807,7 +9546,7 @@
     </row>
     <row r="17" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K18" s="27" t="s">
+      <c r="K18" s="26" t="s">
         <v>75</v>
       </c>
       <c r="L18">
@@ -9833,59 +9572,59 @@
       </c>
     </row>
     <row r="19" spans="6:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K19" s="28" t="s">
+      <c r="K19" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="L19" s="30">
+      <c r="L19" s="29">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="M19" s="30">
+      <c r="M19" s="29">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="N19" s="30">
+      <c r="N19" s="29">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="O19" s="30">
+      <c r="O19" s="29">
         <v>6.4000000000000005E-4</v>
       </c>
-      <c r="P19" s="30">
+      <c r="P19" s="29">
         <v>5.8E-4</v>
       </c>
-      <c r="Q19" s="30">
+      <c r="Q19" s="29">
         <v>5.6999999999999998E-4</v>
       </c>
-      <c r="R19" s="32">
+      <c r="R19" s="31">
         <v>3.8999999999999999E-4</v>
       </c>
     </row>
     <row r="20" spans="6:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K20" s="28" t="s">
+      <c r="K20" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="L20" s="30">
+      <c r="L20" s="29">
         <v>7.46E-2</v>
       </c>
-      <c r="M20" s="30">
+      <c r="M20" s="29">
         <v>5.62E-2</v>
       </c>
-      <c r="N20" s="30">
+      <c r="N20" s="29">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="O20" s="30">
+      <c r="O20" s="29">
         <v>4.1799999999999997E-2</v>
       </c>
-      <c r="P20" s="30">
+      <c r="P20" s="29">
         <v>3.918E-2</v>
       </c>
-      <c r="Q20" s="30">
+      <c r="Q20" s="29">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="R20" s="32">
+      <c r="R20" s="31">
         <v>2.0400000000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="6:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K21" s="28" t="s">
+      <c r="K21" s="27" t="s">
         <v>79</v>
       </c>
       <c r="L21">
@@ -9912,274 +9651,274 @@
     </row>
     <row r="26" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F27" s="42" t="s">
+      <c r="F27" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="G27" s="43">
+      <c r="G27" s="41">
         <v>16000</v>
       </c>
-      <c r="H27" s="43">
+      <c r="H27" s="41">
         <v>27900</v>
       </c>
-      <c r="I27" s="43">
+      <c r="I27" s="41">
         <v>36500</v>
       </c>
-      <c r="J27" s="43">
+      <c r="J27" s="41">
         <v>49600</v>
       </c>
-      <c r="K27" s="43">
+      <c r="K27" s="41">
         <v>57100</v>
       </c>
-      <c r="L27" s="43">
+      <c r="L27" s="41">
         <v>60000</v>
       </c>
-      <c r="M27" s="43">
+      <c r="M27" s="41">
         <v>76600</v>
       </c>
     </row>
     <row r="28" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="44"/>
-      <c r="G28" s="101" t="s">
+      <c r="F28" s="42"/>
+      <c r="G28" s="100" t="s">
         <v>84</v>
       </c>
-      <c r="H28" s="102"/>
-      <c r="I28" s="102"/>
-      <c r="J28" s="102"/>
-      <c r="K28" s="102"/>
-      <c r="L28" s="102"/>
-      <c r="M28" s="103"/>
+      <c r="H28" s="101"/>
+      <c r="I28" s="101"/>
+      <c r="J28" s="101"/>
+      <c r="K28" s="101"/>
+      <c r="L28" s="101"/>
+      <c r="M28" s="102"/>
     </row>
     <row r="29" spans="6:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F29" s="45" t="s">
+      <c r="F29" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="G29" s="46">
+      <c r="G29" s="44">
         <v>1.146E-2</v>
       </c>
-      <c r="H29" s="46">
+      <c r="H29" s="44">
         <v>8.4089999999999998E-3</v>
       </c>
-      <c r="I29" s="46">
+      <c r="I29" s="44">
         <v>7.2880000000000002E-3</v>
       </c>
-      <c r="J29" s="46">
+      <c r="J29" s="44">
         <v>5.7679999999999997E-3</v>
       </c>
-      <c r="K29" s="46">
+      <c r="K29" s="44">
         <v>4.3639999999999998E-3</v>
       </c>
-      <c r="L29" s="46">
+      <c r="L29" s="44">
         <v>3.885E-3</v>
       </c>
-      <c r="M29" s="46">
+      <c r="M29" s="44">
         <v>3.1909999999999998E-3</v>
       </c>
     </row>
     <row r="30" spans="6:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F30" s="45" t="s">
+      <c r="F30" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="46">
+      <c r="G30" s="44">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="H30" s="46">
+      <c r="H30" s="44">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="I30" s="46">
+      <c r="I30" s="44">
         <v>5.2900000000000003E-2</v>
       </c>
-      <c r="J30" s="46">
+      <c r="J30" s="44">
         <v>4.6210000000000001E-2</v>
       </c>
-      <c r="K30" s="46">
+      <c r="K30" s="44">
         <v>4.3380000000000002E-2</v>
       </c>
-      <c r="L30" s="46">
+      <c r="L30" s="44">
         <v>4.2430000000000002E-2</v>
       </c>
-      <c r="M30" s="46">
+      <c r="M30" s="44">
         <v>1.941E-3</v>
       </c>
     </row>
     <row r="31" spans="6:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F31" s="45" t="s">
+      <c r="F31" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="G31" s="46">
+      <c r="G31" s="44">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="H31" s="46">
+      <c r="H31" s="44">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="I31" s="46">
+      <c r="I31" s="44">
         <v>2.5790000000000001E-3</v>
       </c>
-      <c r="J31" s="46">
+      <c r="J31" s="44">
         <v>2.2200000000000002E-3</v>
       </c>
-      <c r="K31" s="46">
+      <c r="K31" s="44">
         <v>2E-3</v>
       </c>
-      <c r="L31" s="46">
+      <c r="L31" s="44">
         <v>1.9980000000000002E-3</v>
       </c>
-      <c r="M31" s="46">
+      <c r="M31" s="44">
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
     <row r="32" spans="6:18" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F32" s="45" t="s">
+      <c r="F32" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="46">
+      <c r="G32" s="44">
         <v>3.4130000000000001E-2</v>
       </c>
-      <c r="H32" s="46">
+      <c r="H32" s="44">
         <v>2.5899999999999999E-2</v>
       </c>
-      <c r="I32" s="46">
+      <c r="I32" s="44">
         <v>2.2710000000000001E-2</v>
       </c>
-      <c r="J32" s="46">
+      <c r="J32" s="44">
         <v>1.95E-2</v>
       </c>
-      <c r="K32" s="46">
+      <c r="K32" s="44">
         <v>1.8180000000000002E-2</v>
       </c>
-      <c r="L32" s="46">
+      <c r="L32" s="44">
         <v>1.7739999999999999E-2</v>
       </c>
-      <c r="M32" s="46">
+      <c r="M32" s="44">
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
     <row r="33" spans="6:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="45" t="s">
+      <c r="F33" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="G33" s="46">
+      <c r="G33" s="44">
         <v>3.7019999999999997E-2</v>
       </c>
-      <c r="H33" s="46">
+      <c r="H33" s="44">
         <v>2.818E-2</v>
       </c>
-      <c r="I33" s="46">
+      <c r="I33" s="44">
         <v>2.4639999999999999E-2</v>
       </c>
-      <c r="J33" s="46">
+      <c r="J33" s="44">
         <v>2.12E-2</v>
       </c>
-      <c r="K33" s="46">
+      <c r="K33" s="44">
         <v>1.9789999999999999E-2</v>
       </c>
-      <c r="L33" s="46">
+      <c r="L33" s="44">
         <v>1.9269999999999999E-2</v>
       </c>
-      <c r="M33" s="46">
+      <c r="M33" s="44">
         <v>6.3099999999999996E-3</v>
       </c>
     </row>
     <row r="34" spans="6:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="45" t="s">
+      <c r="F34" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G34" s="46">
+      <c r="G34" s="44">
         <v>5.4809999999999998E-2</v>
       </c>
-      <c r="H34" s="46">
+      <c r="H34" s="44">
         <v>4.2220000000000001E-2</v>
       </c>
-      <c r="I34" s="46">
+      <c r="I34" s="44">
         <v>3.7100000000000001E-2</v>
       </c>
-      <c r="J34" s="46">
+      <c r="J34" s="44">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="K34" s="46">
+      <c r="K34" s="44">
         <v>2.9940000000000001E-2</v>
       </c>
-      <c r="L34" s="46">
+      <c r="L34" s="44">
         <v>2.92E-2</v>
       </c>
-      <c r="M34" s="46">
+      <c r="M34" s="44">
         <v>4.5199999999999997E-3</v>
       </c>
     </row>
     <row r="35" spans="6:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F35" s="45" t="s">
+      <c r="F35" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="G35" s="46">
+      <c r="G35" s="44">
         <v>2.726E-2</v>
       </c>
-      <c r="H35" s="46">
+      <c r="H35" s="44">
         <v>2.06E-2</v>
       </c>
-      <c r="I35" s="46">
+      <c r="I35" s="44">
         <v>1.8069999999999999E-2</v>
       </c>
-      <c r="J35" s="46">
+      <c r="J35" s="44">
         <v>1.5509999999999999E-2</v>
       </c>
-      <c r="K35" s="46">
+      <c r="K35" s="44">
         <v>1.447E-2</v>
       </c>
-      <c r="L35" s="46">
+      <c r="L35" s="44">
         <v>1.41E-2</v>
       </c>
-      <c r="M35" s="46">
+      <c r="M35" s="44">
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
     <row r="36" spans="6:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F36" s="45" t="s">
+      <c r="F36" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="G36" s="46">
+      <c r="G36" s="44">
         <v>1.4800000000000001E-2</v>
       </c>
-      <c r="H36" s="46">
+      <c r="H36" s="44">
         <v>1.12E-2</v>
       </c>
-      <c r="I36" s="46">
+      <c r="I36" s="44">
         <v>9.7900000000000001E-3</v>
       </c>
-      <c r="J36" s="46">
+      <c r="J36" s="44">
         <v>8.3899999999999999E-3</v>
       </c>
-      <c r="K36" s="46">
+      <c r="K36" s="44">
         <v>7.8189999999999996E-3</v>
       </c>
-      <c r="L36" s="46">
+      <c r="L36" s="44">
         <v>7.62E-3</v>
       </c>
-      <c r="M36" s="46">
+      <c r="M36" s="44">
         <v>4.2069999999999998E-3</v>
       </c>
     </row>
     <row r="37" spans="6:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="45" t="s">
+      <c r="F37" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="G37" s="47">
+      <c r="G37" s="45">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="H37" s="47">
+      <c r="H37" s="45">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="I37" s="47">
+      <c r="I37" s="45">
         <v>7.3600000000000002E-3</v>
       </c>
-      <c r="J37" s="47">
+      <c r="J37" s="45">
         <v>6.3E-3</v>
       </c>
-      <c r="K37" s="47">
+      <c r="K37" s="45">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="L37" s="47">
+      <c r="L37" s="45">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="M37" s="47">
+      <c r="M37" s="45">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
@@ -10469,138 +10208,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="27" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29">
+      <c r="A2" s="28">
         <v>1.051031378</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="29">
         <v>0.25</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="29">
         <v>4</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="29">
         <v>0.53800000000000003</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="29">
         <v>1.4670000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29">
+      <c r="A3" s="28">
         <v>0.225274538</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="29">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="29">
         <v>1.0620000000000001</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="29">
         <v>0.23400000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29">
+      <c r="A4" s="28">
         <v>0.110535912</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="29">
         <v>1.5599999999999999E-2</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="29">
         <v>0.36499999999999999</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="29">
         <v>2.4799999999999999E-2</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="29">
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29">
+      <c r="A5" s="28">
         <v>5.8002663000000003E-2</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="29">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="29">
         <v>0.23100000000000001</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="29">
         <v>1.54E-2</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="29">
+      <c r="A6" s="28">
         <v>3.4605404999999999E-2</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="29">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="29">
         <v>0.16900000000000001</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="29">
         <v>1.1299999999999999E-2</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="29">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29">
+      <c r="A7" s="28">
         <v>2.1080000000000002E-2</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="29">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="29">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="29">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <v>0.03</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31">
+      <c r="A8" s="30">
         <v>2.0655E-2</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="31">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="31">
         <v>0.124</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <v>2.6700000000000002E-2</v>
       </c>
     </row>
@@ -10608,30 +10347,30 @@
       <c r="F10" t="s">
         <v>80</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="35">
         <v>210</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="35">
         <v>1175</v>
       </c>
-      <c r="I10" s="36">
+      <c r="I10" s="35">
         <v>2875</v>
       </c>
-      <c r="J10" s="36">
+      <c r="J10" s="35">
         <v>5275</v>
       </c>
-      <c r="K10" s="36">
+      <c r="K10" s="35">
         <v>7775</v>
       </c>
-      <c r="L10" s="36">
+      <c r="L10" s="35">
         <v>10275</v>
       </c>
-      <c r="M10" s="37">
+      <c r="M10" s="36">
         <v>13775</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="32" t="s">
         <v>75</v>
       </c>
       <c r="G11">
@@ -10657,7 +10396,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="33" t="s">
         <v>61</v>
       </c>
       <c r="G12">
@@ -10683,7 +10422,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="33" t="s">
         <v>66</v>
       </c>
       <c r="G13">
@@ -10707,10 +10446,10 @@
       <c r="M13">
         <v>1.0460000000000001E-2</v>
       </c>
-      <c r="Q13" s="39"/>
+      <c r="Q13" s="37"/>
     </row>
     <row r="14" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="33" t="s">
         <v>62</v>
       </c>
       <c r="G14">
@@ -10734,10 +10473,10 @@
       <c r="M14">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="Q14" s="40"/>
+      <c r="Q14" s="38"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="33" t="s">
         <v>63</v>
       </c>
       <c r="G15">
@@ -10761,10 +10500,10 @@
       <c r="M15">
         <v>9.4E-2</v>
       </c>
-      <c r="Q15" s="40"/>
+      <c r="Q15" s="38"/>
     </row>
     <row r="16" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F16" s="34" t="s">
+      <c r="F16" s="33" t="s">
         <v>64</v>
       </c>
       <c r="G16">
@@ -10788,10 +10527,10 @@
       <c r="M16">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="Q16" s="40"/>
+      <c r="Q16" s="38"/>
     </row>
     <row r="17" spans="6:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="33" t="s">
         <v>65</v>
       </c>
       <c r="G17">
@@ -10815,10 +10554,10 @@
       <c r="M17">
         <v>6.3E-2</v>
       </c>
-      <c r="Q17" s="40"/>
+      <c r="Q17" s="38"/>
     </row>
     <row r="18" spans="6:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="34" t="s">
         <v>67</v>
       </c>
       <c r="G18">
@@ -10842,163 +10581,163 @@
       <c r="M18">
         <v>2.87E-2</v>
       </c>
-      <c r="Q18" s="40"/>
+      <c r="Q18" s="38"/>
     </row>
     <row r="19" spans="6:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="39">
+      <c r="G19" s="37">
         <v>1.4670000000000001</v>
       </c>
-      <c r="H19" s="40">
+      <c r="H19" s="38">
         <v>0.23400000000000001</v>
       </c>
-      <c r="I19" s="40">
+      <c r="I19" s="38">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="J19" s="40">
+      <c r="J19" s="38">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="K19" s="40">
+      <c r="K19" s="38">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="L19" s="40">
+      <c r="L19" s="38">
         <v>0.03</v>
       </c>
-      <c r="M19" s="41">
+      <c r="M19" s="39">
         <v>2.6700000000000002E-2</v>
       </c>
-      <c r="Q19" s="41"/>
+      <c r="Q19" s="39"/>
     </row>
     <row r="22" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="28">
         <v>1.051031378</v>
       </c>
-      <c r="H23" s="29">
+      <c r="H23" s="28">
         <v>0.225274538</v>
       </c>
-      <c r="I23" s="29">
+      <c r="I23" s="28">
         <v>0.110535912</v>
       </c>
-      <c r="J23" s="29">
+      <c r="J23" s="28">
         <v>5.8002663000000003E-2</v>
       </c>
-      <c r="K23" s="29">
+      <c r="K23" s="28">
         <v>3.4605404999999999E-2</v>
       </c>
-      <c r="L23" s="29">
+      <c r="L23" s="28">
         <v>2.1080000000000002E-2</v>
       </c>
-      <c r="M23" s="31">
+      <c r="M23" s="30">
         <v>2.0655E-2</v>
       </c>
     </row>
     <row r="24" spans="6:17" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="30">
+      <c r="G24" s="29">
         <v>0.25</v>
       </c>
-      <c r="H24" s="30">
+      <c r="H24" s="29">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="I24" s="30">
+      <c r="I24" s="29">
         <v>1.5599999999999999E-2</v>
       </c>
-      <c r="J24" s="30">
+      <c r="J24" s="29">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="K24" s="30">
+      <c r="K24" s="29">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="L24" s="30">
+      <c r="L24" s="29">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="M24" s="32">
+      <c r="M24" s="31">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="25" spans="6:17" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="28" t="s">
+      <c r="F25" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G25" s="29">
         <v>4</v>
       </c>
-      <c r="H25" s="30">
+      <c r="H25" s="29">
         <v>1.0620000000000001</v>
       </c>
-      <c r="I25" s="30">
+      <c r="I25" s="29">
         <v>0.36499999999999999</v>
       </c>
-      <c r="J25" s="30">
+      <c r="J25" s="29">
         <v>0.23100000000000001</v>
       </c>
-      <c r="K25" s="30">
+      <c r="K25" s="29">
         <v>0.16900000000000001</v>
       </c>
-      <c r="L25" s="30">
+      <c r="L25" s="29">
         <v>0.14000000000000001</v>
       </c>
-      <c r="M25" s="32">
+      <c r="M25" s="31">
         <v>0.124</v>
       </c>
     </row>
     <row r="26" spans="6:17" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="30">
+      <c r="G26" s="29">
         <v>0.53800000000000003</v>
       </c>
-      <c r="H26" s="30">
+      <c r="H26" s="29">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I26" s="30">
+      <c r="I26" s="29">
         <v>2.4799999999999999E-2</v>
       </c>
-      <c r="J26" s="30">
+      <c r="J26" s="29">
         <v>1.54E-2</v>
       </c>
-      <c r="K26" s="30">
+      <c r="K26" s="29">
         <v>1.1299999999999999E-2</v>
       </c>
-      <c r="L26" s="30">
+      <c r="L26" s="29">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="M26" s="32">
+      <c r="M26" s="31">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="27" spans="6:17" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F27" s="28" t="s">
+      <c r="F27" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="G27" s="30">
+      <c r="G27" s="29">
         <v>1.4670000000000001</v>
       </c>
-      <c r="H27" s="30">
+      <c r="H27" s="29">
         <v>0.23400000000000001</v>
       </c>
-      <c r="I27" s="30">
+      <c r="I27" s="29">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="J27" s="30">
+      <c r="J27" s="29">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="K27" s="30">
+      <c r="K27" s="29">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="L27" s="30">
+      <c r="L27" s="29">
         <v>0.03</v>
       </c>
-      <c r="M27" s="32">
+      <c r="M27" s="31">
         <v>2.6700000000000002E-2</v>
       </c>
     </row>

</xml_diff>